<commit_message>
doc updates to 2.1, remove small2-applimit1, update fixedConfigsSizes.xlsx and tables
Signed-off-by: Benjamin Hoflich <45051453+bhoflich@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/doc/sourceFiles/fixedConfigSizes.xlsx
+++ b/doc/sourceFiles/fixedConfigSizes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hrosenbe/git/opensource/weathervane/doc/sourceFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\git\weathervane\doc\sourceFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BCBA16-93BA-3642-A203-17789750AC1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD3036C-6D9E-4489-938E-0FD9A093B287}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{AF3EA68B-9CB6-DF4D-B5EE-93D818FB3527}"/>
+    <workbookView xWindow="1215" yWindow="1800" windowWidth="21840" windowHeight="12735" xr2:uid="{AF3EA68B-9CB6-DF4D-B5EE-93D818FB3527}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="48">
   <si>
     <t>Weathervane Version:</t>
   </si>
@@ -174,13 +174,13 @@
     <t>Also see this page: https://tableconvert.com/Excel-Converter/excel-to-markdown-table.html</t>
   </si>
   <si>
-    <t>2.0.4</t>
-  </si>
-  <si>
     <t>xsmall</t>
   </si>
   <si>
     <t>small2</t>
+  </si>
+  <si>
+    <t>small2-applimit2</t>
   </si>
 </sst>
 </file>
@@ -515,6 +515,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -524,13 +530,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -989,62 +989,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{250F6D4A-63AF-A141-9CAC-36EA1776C204}">
-  <dimension ref="A1:Y43"/>
+  <dimension ref="A1:AK43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:X20"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AE14" sqref="AE14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B3" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="34" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B3" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="32" t="s">
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="31"/>
+      <c r="V3" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="33"/>
-      <c r="V3" s="35" t="s">
+      <c r="W3" s="31"/>
+      <c r="X3" s="31"/>
+      <c r="Y3" s="31"/>
+      <c r="Z3" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA3" s="31"/>
+      <c r="AB3" s="31"/>
+      <c r="AC3" s="31"/>
+      <c r="AD3" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE3" s="31"/>
+      <c r="AF3" s="31"/>
+      <c r="AG3" s="31"/>
+      <c r="AH3" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="W3" s="33"/>
-      <c r="X3" s="33"/>
-      <c r="Y3" s="33"/>
-    </row>
-    <row r="4" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AI3" s="31"/>
+      <c r="AJ3" s="31"/>
+      <c r="AK3" s="31"/>
+    </row>
+    <row r="4" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1120,8 +1138,20 @@
       <c r="Y4" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AH4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK4" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>12</v>
       </c>
@@ -1183,8 +1213,17 @@
       <c r="X5">
         <v>3700</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AH5" s="1">
+        <v>4</v>
+      </c>
+      <c r="AI5">
+        <v>700</v>
+      </c>
+      <c r="AJ5">
+        <v>3700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1246,8 +1285,17 @@
       <c r="X6">
         <v>1500</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AH6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI6">
+        <v>300</v>
+      </c>
+      <c r="AJ6">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>14</v>
       </c>
@@ -1311,8 +1359,18 @@
         <v>16300</v>
       </c>
       <c r="Y7" s="7"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AH7" s="6"/>
+      <c r="AI7" s="7">
+        <f>SUM(AH5*AI5,AH6*AI6)/1000</f>
+        <v>3.1</v>
+      </c>
+      <c r="AJ7" s="7">
+        <f>SUM(AH5*AJ5,AH6*AJ6)</f>
+        <v>16300</v>
+      </c>
+      <c r="AK7" s="7"/>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1389,8 +1447,20 @@
       <c r="Y8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AH8" s="1">
+        <v>2</v>
+      </c>
+      <c r="AI8">
+        <v>780</v>
+      </c>
+      <c r="AJ8">
+        <v>5500</v>
+      </c>
+      <c r="AK8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1452,8 +1522,17 @@
       <c r="X9">
         <v>5000</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AH9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI9">
+        <v>2000</v>
+      </c>
+      <c r="AJ9">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1516,8 +1595,17 @@
       <c r="X10">
         <v>6000</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AH10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI10">
+        <v>1950</v>
+      </c>
+      <c r="AJ10">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1580,8 +1668,17 @@
       <c r="X11">
         <v>100</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AH11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI11">
+        <v>20</v>
+      </c>
+      <c r="AJ11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1643,8 +1740,17 @@
       <c r="X12">
         <v>500</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AH12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI12">
+        <v>150</v>
+      </c>
+      <c r="AJ12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
@@ -1720,8 +1826,20 @@
       <c r="Y13">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AH13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI13">
+        <v>500</v>
+      </c>
+      <c r="AJ13">
+        <v>4000</v>
+      </c>
+      <c r="AK13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -1798,8 +1916,20 @@
       <c r="Y14">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AH14" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI14">
+        <v>780</v>
+      </c>
+      <c r="AJ14">
+        <v>6000</v>
+      </c>
+      <c r="AK14">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>22</v>
       </c>
@@ -1884,8 +2014,21 @@
         <f>SUM(V8*Y8,V13*Y13,V14*Y14)</f>
         <v>80</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AH15" s="6"/>
+      <c r="AI15" s="7">
+        <f>SUM(AH8*AI8,AH9*AI9,AH10*AI10,AH11*AI11,AH12*AI12,AH13*AI13,AH14*AI14)/1000</f>
+        <v>6.96</v>
+      </c>
+      <c r="AJ15" s="7">
+        <f>SUM(AH8*AJ8,AH9*AJ9,AH10*AJ10,AH11*AJ11,AH12*AJ12,AH13*AJ13,AH14*AJ14)</f>
+        <v>32600</v>
+      </c>
+      <c r="AK15" s="7">
+        <f>SUM(AH8*AK8,AH13*AK13,AH14*AK14)</f>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="E16" s="2"/>
       <c r="F16" s="1"/>
@@ -1898,8 +2041,10 @@
       <c r="U16" s="2"/>
       <c r="V16" s="1"/>
       <c r="Y16" s="2"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AH16" s="1"/>
+      <c r="AK16" s="2"/>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1981,59 +2126,72 @@
         <f>Y15</f>
         <v>80</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AH17" s="12"/>
+      <c r="AI17" s="13">
+        <f>AI7+AI15</f>
+        <v>10.06</v>
+      </c>
+      <c r="AJ17" s="13">
+        <f>AJ7+AJ15</f>
+        <v>48900</v>
+      </c>
+      <c r="AK17" s="14">
+        <f>AK15</f>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="L18" s="26"/>
       <c r="X18" s="26"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="L19" s="26"/>
       <c r="X19" s="26"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="L20" s="26"/>
       <c r="X20" s="26"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B22" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="30" t="s">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B22" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="33"/>
+      <c r="D22" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="31"/>
-      <c r="F22" s="30" t="s">
+      <c r="E22" s="33"/>
+      <c r="F22" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22" s="33"/>
+      <c r="H22" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="I22" s="33"/>
+      <c r="J22" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="K22" s="33"/>
+      <c r="L22" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="31"/>
-      <c r="H22" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="I22" s="31"/>
-      <c r="J22" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="K22" s="31"/>
-      <c r="L22" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="M22" s="31"/>
-      <c r="N22" s="30" t="s">
+      <c r="M22" s="33"/>
+      <c r="N22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="O22" s="31"/>
-      <c r="P22" s="30" t="s">
+      <c r="O22" s="33"/>
+      <c r="P22" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="Q22" s="31"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Q22" s="33"/>
+    </row>
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -2086,7 +2244,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2155,7 +2313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25">
         <f>A24+1</f>
         <v>2</v>
@@ -2225,7 +2383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" ref="A26:A43" si="8">A25+1</f>
         <v>3</v>
@@ -2295,7 +2453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="8"/>
         <v>4</v>
@@ -2365,7 +2523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="8"/>
         <v>5</v>
@@ -2435,7 +2593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="8"/>
         <v>6</v>
@@ -2505,7 +2663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="8"/>
         <v>7</v>
@@ -2575,7 +2733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="8"/>
         <v>8</v>
@@ -2645,7 +2803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="8"/>
         <v>9</v>
@@ -2715,7 +2873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="8"/>
         <v>10</v>
@@ -2785,7 +2943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="8"/>
         <v>11</v>
@@ -2855,7 +3013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="8"/>
         <v>12</v>
@@ -2925,7 +3083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="8"/>
         <v>13</v>
@@ -2995,7 +3153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="8"/>
         <v>14</v>
@@ -3065,7 +3223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="8"/>
         <v>15</v>
@@ -3135,7 +3293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="8"/>
         <v>16</v>
@@ -3205,7 +3363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="8"/>
         <v>17</v>
@@ -3275,7 +3433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="8"/>
         <v>18</v>
@@ -3345,7 +3503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="8"/>
         <v>19</v>
@@ -3415,7 +3573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="8"/>
         <v>20</v>
@@ -3486,21 +3644,24 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="17">
+    <mergeCell ref="L22:M22"/>
     <mergeCell ref="V3:Y3"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="N3:Q3"/>
     <mergeCell ref="R3:U3"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="P22:Q22"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="J22:K22"/>
-    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="Z3:AC3"/>
+    <mergeCell ref="AD3:AG3"/>
+    <mergeCell ref="AH3:AK3"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:Q22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3508,27 +3669,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9404EA0-BEB2-2D4D-AB49-307F1D632573}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>28</v>
       </c>
@@ -3539,16 +3700,16 @@
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
       <c r="F1" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G1" s="21"/>
       <c r="H1" s="21"/>
       <c r="I1" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J1" s="21"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
       <c r="B2" s="24" t="s">
         <v>9</v>
@@ -3578,7 +3739,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>14</v>
       </c>
@@ -3586,7 +3747,7 @@
         <f>data!C7</f>
         <v>0.5</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="23">
         <f>(data!D7)/1024</f>
         <v>1.66015625</v>
       </c>
@@ -3598,7 +3759,7 @@
         <f>data!K7</f>
         <v>2.5499999999999998</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="23">
         <f>data!L7/1024</f>
         <v>9.375</v>
       </c>
@@ -3610,7 +3771,7 @@
         <f>data!W7</f>
         <v>3.1</v>
       </c>
-      <c r="I3" s="29">
+      <c r="I3" s="23">
         <f>data!X7/1024</f>
         <v>15.91796875</v>
       </c>
@@ -3619,7 +3780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>22</v>
       </c>
@@ -3627,7 +3788,7 @@
         <f>data!C15</f>
         <v>0.79100000000000004</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="23">
         <f>(data!D15)/1024</f>
         <v>5.56640625</v>
       </c>
@@ -3639,7 +3800,7 @@
         <f>data!K15</f>
         <v>2.59</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="23">
         <f>data!L15/1024</f>
         <v>12.509765625</v>
       </c>
@@ -3651,7 +3812,7 @@
         <f>data!W15</f>
         <v>4.8</v>
       </c>
-      <c r="I4" s="29">
+      <c r="I4" s="23">
         <f>data!X15/1024</f>
         <v>31.8359375</v>
       </c>
@@ -3660,39 +3821,39 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="23">
-        <f>B4+B3</f>
+        <f t="shared" ref="B5:H5" si="0">B4+B3</f>
         <v>1.2909999999999999</v>
       </c>
-      <c r="C5" s="29">
-        <f>C4+C3</f>
+      <c r="C5" s="23">
+        <f t="shared" si="0"/>
         <v>7.2265625</v>
       </c>
       <c r="D5" s="23">
-        <f>D4+D3</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="E5" s="23">
-        <f>E4+E3</f>
+        <f t="shared" si="0"/>
         <v>5.14</v>
       </c>
-      <c r="F5" s="29">
-        <f>F4+F3</f>
+      <c r="F5" s="23">
+        <f t="shared" si="0"/>
         <v>21.884765625</v>
       </c>
       <c r="G5" s="23">
-        <f>G4+G3</f>
+        <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="H5" s="29">
-        <f>H4+H3</f>
+      <c r="H5" s="23">
+        <f t="shared" si="0"/>
         <v>7.9</v>
       </c>
-      <c r="I5" s="29">
+      <c r="I5" s="23">
         <f>I3+I4</f>
         <v>47.75390625</v>
       </c>
@@ -3701,8 +3862,112 @@
         <v>80</v>
       </c>
     </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="23">
+        <f>data!AI7</f>
+        <v>3.1</v>
+      </c>
+      <c r="C11" s="23">
+        <f>data!AJ7/1024</f>
+        <v>15.91796875</v>
+      </c>
+      <c r="D11" s="23">
+        <f>data!AK7</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="23">
+        <f>data!AI15</f>
+        <v>6.96</v>
+      </c>
+      <c r="C12" s="23">
+        <f>data!AJ15/1024</f>
+        <v>31.8359375</v>
+      </c>
+      <c r="D12" s="23">
+        <f>data!AK15</f>
+        <v>87</v>
+      </c>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="23">
+        <f t="shared" ref="B13:D13" si="1">B12+B11</f>
+        <v>10.06</v>
+      </c>
+      <c r="C13" s="23">
+        <f>C11+C12</f>
+        <v>47.75390625</v>
+      </c>
+      <c r="D13" s="23">
+        <f>D11+D12</f>
+        <v>87</v>
+      </c>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3711,15 +3976,15 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection sqref="A1:J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>28</v>
       </c>
@@ -3730,16 +3995,16 @@
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
       <c r="F1" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G1" s="21"/>
       <c r="H1" s="21"/>
       <c r="I1" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J1" s="21"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>27</v>
       </c>
@@ -3771,7 +4036,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <v>1</v>
       </c>
@@ -3812,7 +4077,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
         <v>2</v>
       </c>
@@ -3853,7 +4118,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <v>3</v>
       </c>
@@ -3894,7 +4159,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
         <v>4</v>
       </c>
@@ -3935,7 +4200,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
         <v>5</v>
       </c>
@@ -3976,7 +4241,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
         <v>6</v>
       </c>
@@ -4017,7 +4282,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="21">
         <v>7</v>
       </c>
@@ -4058,7 +4323,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
         <v>8</v>
       </c>
@@ -4099,7 +4364,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
         <v>9</v>
       </c>
@@ -4140,7 +4405,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <v>10</v>
       </c>
@@ -4181,7 +4446,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="21">
         <v>11</v>
       </c>
@@ -4222,7 +4487,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
         <v>12</v>
       </c>
@@ -4263,7 +4528,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="21">
         <v>13</v>
       </c>
@@ -4304,7 +4569,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
         <v>14</v>
       </c>
@@ -4345,7 +4610,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="21">
         <v>15</v>
       </c>
@@ -4386,7 +4651,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="21">
         <v>16</v>
       </c>
@@ -4427,7 +4692,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="21">
         <v>17</v>
       </c>
@@ -4468,7 +4733,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="21">
         <v>18</v>
       </c>
@@ -4509,7 +4774,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="21">
         <v>19</v>
       </c>
@@ -4550,7 +4815,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="21">
         <v>20</v>
       </c>
@@ -4601,15 +4866,15 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>28</v>
       </c>
@@ -4620,16 +4885,16 @@
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
       <c r="F1" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G1" s="21"/>
       <c r="H1" s="21"/>
       <c r="I1" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J1" s="21"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>27</v>
       </c>
@@ -4661,7 +4926,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <v>1</v>
       </c>
@@ -4701,7 +4966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
         <v>2</v>
       </c>
@@ -4741,7 +5006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <v>3</v>
       </c>
@@ -4781,7 +5046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
         <v>4</v>
       </c>
@@ -4821,7 +5086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
         <v>5</v>
       </c>
@@ -4861,7 +5126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
         <v>6</v>
       </c>
@@ -4901,7 +5166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="21">
         <v>7</v>
       </c>
@@ -4941,7 +5206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
         <v>8</v>
       </c>
@@ -4981,7 +5246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
         <v>9</v>
       </c>
@@ -5021,7 +5286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <v>10</v>
       </c>
@@ -5061,7 +5326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="21">
         <v>11</v>
       </c>
@@ -5101,7 +5366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
         <v>12</v>
       </c>
@@ -5141,7 +5406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="21">
         <v>13</v>
       </c>
@@ -5181,7 +5446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
         <v>14</v>
       </c>
@@ -5221,7 +5486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="21">
         <v>15</v>
       </c>
@@ -5261,7 +5526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="21">
         <v>16</v>
       </c>
@@ -5301,7 +5566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="21">
         <v>17</v>
       </c>
@@ -5341,7 +5606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="21">
         <v>18</v>
       </c>
@@ -5381,7 +5646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="21">
         <v>19</v>
       </c>
@@ -5421,7 +5686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="21">
         <v>20</v>
       </c>
@@ -5470,28 +5735,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{616FE546-8080-2A45-A22C-2BF119538D85}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>30</v>
       </c>
@@ -5499,47 +5764,47 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Updating excel file. Signed-off-by: Luis Alvarez Sanchez <lalvarezsanc@vmware.com>
</commit_message>
<xml_diff>
--- a/doc/sourceFiles/fixedConfigSizes.xlsx
+++ b/doc/sourceFiles/fixedConfigSizes.xlsx
@@ -138,7 +138,7 @@
       <rPr>
         <u val="single"/>
         <sz val="12"/>
-        <color indexed="11"/>
+        <color indexed="12"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>https://tableconvert.com/</t>
@@ -209,11 +209,11 @@
     <font>
       <u val="single"/>
       <sz val="12"/>
-      <color indexed="11"/>
+      <color indexed="12"/>
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,7 +222,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="11"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -237,28 +243,28 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="medium">
         <color indexed="8"/>
@@ -267,16 +273,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="medium">
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -285,34 +291,34 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="medium">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="medium">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="medium">
         <color indexed="8"/>
@@ -321,13 +327,13 @@
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
@@ -336,7 +342,7 @@
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -345,25 +351,25 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="medium">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="medium">
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="8"/>
@@ -375,10 +381,10 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="medium">
         <color indexed="8"/>
@@ -387,13 +393,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="medium">
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="medium">
         <color indexed="8"/>
@@ -402,13 +408,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="medium">
         <color indexed="8"/>
@@ -420,10 +426,10 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="medium">
         <color indexed="8"/>
@@ -432,16 +438,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -456,7 +462,7 @@
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -468,7 +474,7 @@
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="medium">
         <color indexed="8"/>
@@ -495,7 +501,7 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="medium">
         <color indexed="8"/>
@@ -507,10 +513,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="medium">
         <color indexed="8"/>
@@ -522,7 +528,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
@@ -546,7 +552,7 @@
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -558,10 +564,10 @@
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -570,13 +576,13 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -600,7 +606,7 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="medium">
         <color indexed="8"/>
@@ -612,7 +618,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="medium">
         <color indexed="8"/>
@@ -630,10 +636,10 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="8"/>
@@ -642,13 +648,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="8"/>
@@ -657,13 +663,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="8"/>
@@ -678,7 +684,7 @@
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="8"/>
@@ -687,16 +693,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -705,19 +711,19 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
@@ -726,7 +732,7 @@
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -735,7 +741,7 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
@@ -747,7 +753,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
@@ -762,11 +768,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -775,7 +781,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -783,17 +789,17 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top/>
@@ -810,7 +816,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom/>
@@ -818,38 +824,38 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -858,18 +864,18 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -886,289 +892,289 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="30" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="2" fontId="0" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="2" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="33" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="60" fontId="0" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="60" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="60" fontId="0" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="60" fontId="0" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="60" fontId="0" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="60" fontId="0" fillId="2" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="42" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="43" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="43" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="40" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="41" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="61" fontId="0" fillId="2" borderId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="61" fontId="0" fillId="3" borderId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="3" borderId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="3" borderId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="3" borderId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="3" borderId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1194,6 +1200,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="fffff2cb"/>
       <rgbColor rgb="ff0563c1"/>
@@ -1535,17 +1542,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1573,10 +1580,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1824,12 +1831,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -2116,7 +2123,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2144,10 +2151,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -3459,7 +3466,7 @@
         <v>1000</v>
       </c>
       <c r="E13" s="40">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F13" s="37">
         <v>1</v>
@@ -3569,7 +3576,7 @@
         <v>1500</v>
       </c>
       <c r="E14" s="41">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F14" s="26">
         <v>1</v>
@@ -3681,7 +3688,7 @@
       </c>
       <c r="E15" s="44">
         <f>SUM(B8*E8,B13*E13,B14*E14)</f>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F15" s="43"/>
       <c r="G15" s="31">
@@ -3846,7 +3853,7 @@
       </c>
       <c r="E17" s="53">
         <f>E15</f>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F17" s="51"/>
       <c r="G17" s="52">
@@ -7026,7 +7033,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="80">
-        <f>'data'!W7</f>
+        <f>'data'!AM7</f>
         <v>3.1</v>
       </c>
       <c r="I3" s="80">
@@ -7052,7 +7059,7 @@
       </c>
       <c r="D4" s="80">
         <f>'data'!E15</f>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E4" s="80">
         <f>'data'!K15</f>
@@ -7067,8 +7074,8 @@
         <v>59</v>
       </c>
       <c r="H4" s="80">
-        <f>'data'!W15</f>
-        <v>4.8</v>
+        <f>'data'!AM15</f>
+        <v>6.91</v>
       </c>
       <c r="I4" s="80">
         <f>'data'!AN15/1024</f>
@@ -7093,7 +7100,7 @@
       </c>
       <c r="D5" s="80">
         <f>D4+D3</f>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E5" s="80">
         <f>E4+E3</f>
@@ -7109,7 +7116,7 @@
       </c>
       <c r="H5" s="80">
         <f>H4+H3</f>
-        <v>7.9</v>
+        <v>10.01</v>
       </c>
       <c r="I5" s="80">
         <f>I3+I4</f>
@@ -7304,7 +7311,7 @@
       </c>
       <c r="D3" s="92">
         <f>$A3*'Table1'!D$4</f>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E3" s="92">
         <f>$A3*'Table1'!E$4</f>
@@ -7320,7 +7327,7 @@
       </c>
       <c r="H3" s="92">
         <f>$A3*'Table1'!H$4</f>
-        <v>4.8</v>
+        <v>6.91</v>
       </c>
       <c r="I3" s="92">
         <f>$A3*'Table1'!I$4</f>
@@ -7345,7 +7352,7 @@
       </c>
       <c r="D4" s="92">
         <f>$A4*'Table1'!D$4</f>
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="E4" s="92">
         <f>$A4*'Table1'!E$4</f>
@@ -7361,7 +7368,7 @@
       </c>
       <c r="H4" s="92">
         <f>$A4*'Table1'!H$4</f>
-        <v>9.6</v>
+        <v>13.82</v>
       </c>
       <c r="I4" s="92">
         <f>$A4*'Table1'!I$4</f>
@@ -7386,7 +7393,7 @@
       </c>
       <c r="D5" s="92">
         <f>$A5*'Table1'!D$4</f>
-        <v>96</v>
+        <v>48</v>
       </c>
       <c r="E5" s="92">
         <f>$A5*'Table1'!E$4</f>
@@ -7402,7 +7409,7 @@
       </c>
       <c r="H5" s="92">
         <f>$A5*'Table1'!H$4</f>
-        <v>14.4</v>
+        <v>20.73</v>
       </c>
       <c r="I5" s="92">
         <f>$A5*'Table1'!I$4</f>
@@ -7427,7 +7434,7 @@
       </c>
       <c r="D6" s="92">
         <f>$A6*'Table1'!D$4</f>
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="E6" s="92">
         <f>$A6*'Table1'!E$4</f>
@@ -7443,7 +7450,7 @@
       </c>
       <c r="H6" s="92">
         <f>$A6*'Table1'!H$4</f>
-        <v>19.2</v>
+        <v>27.64</v>
       </c>
       <c r="I6" s="92">
         <f>$A6*'Table1'!I$4</f>
@@ -7468,7 +7475,7 @@
       </c>
       <c r="D7" s="92">
         <f>$A7*'Table1'!D$4</f>
-        <v>160</v>
+        <v>80</v>
       </c>
       <c r="E7" s="92">
         <f>$A7*'Table1'!E$4</f>
@@ -7484,7 +7491,7 @@
       </c>
       <c r="H7" s="92">
         <f>$A7*'Table1'!H$4</f>
-        <v>24</v>
+        <v>34.55</v>
       </c>
       <c r="I7" s="92">
         <f>$A7*'Table1'!I$4</f>
@@ -7509,7 +7516,7 @@
       </c>
       <c r="D8" s="92">
         <f>$A8*'Table1'!D$4</f>
-        <v>192</v>
+        <v>96</v>
       </c>
       <c r="E8" s="92">
         <f>$A8*'Table1'!E$4</f>
@@ -7525,7 +7532,7 @@
       </c>
       <c r="H8" s="92">
         <f>$A8*'Table1'!H$4</f>
-        <v>28.8</v>
+        <v>41.46</v>
       </c>
       <c r="I8" s="92">
         <f>$A8*'Table1'!I$4</f>
@@ -7550,7 +7557,7 @@
       </c>
       <c r="D9" s="92">
         <f>$A9*'Table1'!D$4</f>
-        <v>224</v>
+        <v>112</v>
       </c>
       <c r="E9" s="92">
         <f>$A9*'Table1'!E$4</f>
@@ -7566,7 +7573,7 @@
       </c>
       <c r="H9" s="92">
         <f>$A9*'Table1'!H$4</f>
-        <v>33.6</v>
+        <v>48.37</v>
       </c>
       <c r="I9" s="92">
         <f>$A9*'Table1'!I$4</f>
@@ -7591,7 +7598,7 @@
       </c>
       <c r="D10" s="92">
         <f>$A10*'Table1'!D$4</f>
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="E10" s="92">
         <f>$A10*'Table1'!E$4</f>
@@ -7607,7 +7614,7 @@
       </c>
       <c r="H10" s="92">
         <f>$A10*'Table1'!H$4</f>
-        <v>38.4</v>
+        <v>55.28</v>
       </c>
       <c r="I10" s="92">
         <f>$A10*'Table1'!I$4</f>
@@ -7632,7 +7639,7 @@
       </c>
       <c r="D11" s="92">
         <f>$A11*'Table1'!D$4</f>
-        <v>288</v>
+        <v>144</v>
       </c>
       <c r="E11" s="92">
         <f>$A11*'Table1'!E$4</f>
@@ -7648,7 +7655,7 @@
       </c>
       <c r="H11" s="92">
         <f>$A11*'Table1'!H$4</f>
-        <v>43.2</v>
+        <v>62.19</v>
       </c>
       <c r="I11" s="92">
         <f>$A11*'Table1'!I$4</f>
@@ -7673,7 +7680,7 @@
       </c>
       <c r="D12" s="92">
         <f>$A12*'Table1'!D$4</f>
-        <v>320</v>
+        <v>160</v>
       </c>
       <c r="E12" s="92">
         <f>$A12*'Table1'!E$4</f>
@@ -7689,7 +7696,7 @@
       </c>
       <c r="H12" s="92">
         <f>$A12*'Table1'!H$4</f>
-        <v>48</v>
+        <v>69.09999999999999</v>
       </c>
       <c r="I12" s="92">
         <f>$A12*'Table1'!I$4</f>
@@ -7714,7 +7721,7 @@
       </c>
       <c r="D13" s="92">
         <f>$A13*'Table1'!D$4</f>
-        <v>352</v>
+        <v>176</v>
       </c>
       <c r="E13" s="92">
         <f>$A13*'Table1'!E$4</f>
@@ -7730,7 +7737,7 @@
       </c>
       <c r="H13" s="92">
         <f>$A13*'Table1'!H$4</f>
-        <v>52.8</v>
+        <v>76.01000000000001</v>
       </c>
       <c r="I13" s="92">
         <f>$A13*'Table1'!I$4</f>
@@ -7755,7 +7762,7 @@
       </c>
       <c r="D14" s="92">
         <f>$A14*'Table1'!D$4</f>
-        <v>384</v>
+        <v>192</v>
       </c>
       <c r="E14" s="92">
         <f>$A14*'Table1'!E$4</f>
@@ -7771,7 +7778,7 @@
       </c>
       <c r="H14" s="92">
         <f>$A14*'Table1'!H$4</f>
-        <v>57.6</v>
+        <v>82.92</v>
       </c>
       <c r="I14" s="92">
         <f>$A14*'Table1'!I$4</f>
@@ -7796,7 +7803,7 @@
       </c>
       <c r="D15" s="92">
         <f>$A15*'Table1'!D$4</f>
-        <v>416</v>
+        <v>208</v>
       </c>
       <c r="E15" s="92">
         <f>$A15*'Table1'!E$4</f>
@@ -7812,7 +7819,7 @@
       </c>
       <c r="H15" s="92">
         <f>$A15*'Table1'!H$4</f>
-        <v>62.4</v>
+        <v>89.83</v>
       </c>
       <c r="I15" s="92">
         <f>$A15*'Table1'!I$4</f>
@@ -7837,7 +7844,7 @@
       </c>
       <c r="D16" s="92">
         <f>$A16*'Table1'!D$4</f>
-        <v>448</v>
+        <v>224</v>
       </c>
       <c r="E16" s="92">
         <f>$A16*'Table1'!E$4</f>
@@ -7853,7 +7860,7 @@
       </c>
       <c r="H16" s="92">
         <f>$A16*'Table1'!H$4</f>
-        <v>67.2</v>
+        <v>96.73999999999999</v>
       </c>
       <c r="I16" s="92">
         <f>$A16*'Table1'!I$4</f>
@@ -7878,7 +7885,7 @@
       </c>
       <c r="D17" s="92">
         <f>$A17*'Table1'!D$4</f>
-        <v>480</v>
+        <v>240</v>
       </c>
       <c r="E17" s="92">
         <f>$A17*'Table1'!E$4</f>
@@ -7894,7 +7901,7 @@
       </c>
       <c r="H17" s="92">
         <f>$A17*'Table1'!H$4</f>
-        <v>72</v>
+        <v>103.65</v>
       </c>
       <c r="I17" s="92">
         <f>$A17*'Table1'!I$4</f>
@@ -7919,7 +7926,7 @@
       </c>
       <c r="D18" s="92">
         <f>$A18*'Table1'!D$4</f>
-        <v>512</v>
+        <v>256</v>
       </c>
       <c r="E18" s="92">
         <f>$A18*'Table1'!E$4</f>
@@ -7935,7 +7942,7 @@
       </c>
       <c r="H18" s="92">
         <f>$A18*'Table1'!H$4</f>
-        <v>76.8</v>
+        <v>110.56</v>
       </c>
       <c r="I18" s="92">
         <f>$A18*'Table1'!I$4</f>
@@ -7960,7 +7967,7 @@
       </c>
       <c r="D19" s="92">
         <f>$A19*'Table1'!D$4</f>
-        <v>544</v>
+        <v>272</v>
       </c>
       <c r="E19" s="92">
         <f>$A19*'Table1'!E$4</f>
@@ -7976,7 +7983,7 @@
       </c>
       <c r="H19" s="92">
         <f>$A19*'Table1'!H$4</f>
-        <v>81.59999999999999</v>
+        <v>117.47</v>
       </c>
       <c r="I19" s="92">
         <f>$A19*'Table1'!I$4</f>
@@ -8001,7 +8008,7 @@
       </c>
       <c r="D20" s="92">
         <f>$A20*'Table1'!D$4</f>
-        <v>576</v>
+        <v>288</v>
       </c>
       <c r="E20" s="92">
         <f>$A20*'Table1'!E$4</f>
@@ -8017,7 +8024,7 @@
       </c>
       <c r="H20" s="92">
         <f>$A20*'Table1'!H$4</f>
-        <v>86.40000000000001</v>
+        <v>124.38</v>
       </c>
       <c r="I20" s="92">
         <f>$A20*'Table1'!I$4</f>
@@ -8042,7 +8049,7 @@
       </c>
       <c r="D21" s="92">
         <f>$A21*'Table1'!D$4</f>
-        <v>608</v>
+        <v>304</v>
       </c>
       <c r="E21" s="92">
         <f>$A21*'Table1'!E$4</f>
@@ -8058,7 +8065,7 @@
       </c>
       <c r="H21" s="92">
         <f>$A21*'Table1'!H$4</f>
-        <v>91.2</v>
+        <v>131.29</v>
       </c>
       <c r="I21" s="92">
         <f>$A21*'Table1'!I$4</f>
@@ -8083,7 +8090,7 @@
       </c>
       <c r="D22" s="95">
         <f>$A22*'Table1'!D$4</f>
-        <v>640</v>
+        <v>320</v>
       </c>
       <c r="E22" s="95">
         <f>$A22*'Table1'!E$4</f>
@@ -8099,7 +8106,7 @@
       </c>
       <c r="H22" s="95">
         <f>$A22*'Table1'!H$4</f>
-        <v>96</v>
+        <v>138.2</v>
       </c>
       <c r="I22" s="95">
         <f>$A22*'Table1'!I$4</f>

</xml_diff>